<commit_message>
Change from "actual use" to "BOR Consumptive Use & Losses Reports"
</commit_message>
<xml_diff>
--- a/UpperBasinConsumptiveUses/(1) Upper Colorado River Basin Depletions and Evaporation.xlsx
+++ b/UpperBasinConsumptiveUses/(1) Upper Colorado River Basin Depletions and Evaporation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Future_of_the_Colorado_River_Project\UpperBasinConsumptiveUses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C9C29B-42FC-43EE-83ED-53E232889F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC917C33-D325-4845-B110-22FA9EF9DADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="858" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="858" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="14" r:id="rId1"/>
@@ -9154,7 +9154,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{11B20905-5AD1-46D3-BB6C-D0E37E3469F5}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9165,7 +9165,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656674" cy="6282070"/>
+    <xdr:ext cx="8656320" cy="6278880"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -9849,8 +9849,40 @@
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1"/>
-            <a:t>Actual use</a:t>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BOR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Consumptive Use &amp; Losses Reports</a:t>
           </a:r>
         </a:p>
       </cdr:txBody>
@@ -10931,10 +10963,65 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1"/>
-            <a:t>Actual CRSP Reservoir Evaporation</a:t>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BOR</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Consumptive Use &amp; Losses Reports</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:endParaRPr lang="en-US" sz="1200" b="1"/>
@@ -13629,7 +13716,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABA40DF-0866-47B6-B050-3425248E9CA3}">
   <dimension ref="A1:Q219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>

</xml_diff>